<commit_message>
progress on qc checks
</commit_message>
<xml_diff>
--- a/results/qc_check_sheets/qc_check_debrief_and_errors.xlsx
+++ b/results/qc_check_sheets/qc_check_debrief_and_errors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\levan\GitHub\fast_schema_analysis_2\results\qc_check_sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{881C7B0F-3DB7-48A3-9536-903B67149499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6D42EAA-6E08-40EA-BEC6-88AA2D5E0E51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3384" yWindow="3384" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,9 +30,6 @@
     <t>participant</t>
   </si>
   <si>
-    <t>qc_fail</t>
-  </si>
-  <si>
     <t>reason</t>
   </si>
   <si>
@@ -40,6 +37,9 @@
   </si>
   <si>
     <t>sub_002</t>
+  </si>
+  <si>
+    <t>qc_fail_manual</t>
   </si>
 </sst>
 </file>
@@ -360,13 +360,13 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -374,15 +374,15 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" t="b">
         <v>0</v>
@@ -390,7 +390,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
added counterbalancing as info
</commit_message>
<xml_diff>
--- a/results/qc_check_sheets/qc_check_debrief_and_errors.xlsx
+++ b/results/qc_check_sheets/qc_check_debrief_and_errors.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\levan\GitHub\fast_schema_analysis_2\results\qc_check_sheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lb08\GitHub\fast_schema_analysis_2\results\qc_check_sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6D42EAA-6E08-40EA-BEC6-88AA2D5E0E51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3384" yWindow="3384" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3390" yWindow="3390" windowWidth="17280" windowHeight="8970"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>participant</t>
   </si>
@@ -40,12 +39,15 @@
   </si>
   <si>
     <t>qc_fail_manual</t>
+  </si>
+  <si>
+    <t>sub_003</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -356,20 +358,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -380,7 +382,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -388,11 +390,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
new data and now saving display info
</commit_message>
<xml_diff>
--- a/results/qc_check_sheets/qc_check_debrief_and_errors.xlsx
+++ b/results/qc_check_sheets/qc_check_debrief_and_errors.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>participant</t>
   </si>
@@ -42,6 +42,12 @@
   </si>
   <si>
     <t>sub_003</t>
+  </si>
+  <si>
+    <t>sub_004</t>
+  </si>
+  <si>
+    <t>sub_005</t>
   </si>
 </sst>
 </file>
@@ -359,10 +365,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -406,6 +412,22 @@
         <v>0</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
downloaded the new data and analyzing. Added explicit check for scrolling
</commit_message>
<xml_diff>
--- a/results/qc_check_sheets/qc_check_debrief_and_errors.xlsx
+++ b/results/qc_check_sheets/qc_check_debrief_and_errors.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>participant</t>
   </si>
@@ -48,6 +48,21 @@
   </si>
   <si>
     <t>sub_005</t>
+  </si>
+  <si>
+    <t>sub_006</t>
+  </si>
+  <si>
+    <t>sub_007</t>
+  </si>
+  <si>
+    <t>sub_008</t>
+  </si>
+  <si>
+    <t>sub_009</t>
+  </si>
+  <si>
+    <t>sub_010</t>
   </si>
 </sst>
 </file>
@@ -365,10 +380,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -428,6 +443,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
new data downloaded and analyzed
</commit_message>
<xml_diff>
--- a/results/qc_check_sheets/qc_check_debrief_and_errors.xlsx
+++ b/results/qc_check_sheets/qc_check_debrief_and_errors.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lb08\GitHub\fast_schema_analysis_2\results\qc_check_sheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\levan\GitHub\fast_schema_analysis_2\results\qc_check_sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00435A46-39BD-47DF-AFC6-04D90E2316BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3390" yWindow="3390" windowWidth="17280" windowHeight="8970"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>participant</t>
   </si>
@@ -63,16 +64,52 @@
   </si>
   <si>
     <t>sub_010</t>
+  </si>
+  <si>
+    <t>sub_011</t>
+  </si>
+  <si>
+    <t>sub_012</t>
+  </si>
+  <si>
+    <t>sub_013</t>
+  </si>
+  <si>
+    <t>sub_014</t>
+  </si>
+  <si>
+    <t>sub_015</t>
+  </si>
+  <si>
+    <t>sub_016</t>
+  </si>
+  <si>
+    <t>sub_017</t>
+  </si>
+  <si>
+    <t>sub_018</t>
+  </si>
+  <si>
+    <t>sub_019</t>
+  </si>
+  <si>
+    <t>sub_020</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -379,20 +416,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -403,7 +440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -411,7 +448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -419,7 +456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -427,7 +464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -435,7 +472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -443,7 +480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -451,7 +488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -459,7 +496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -467,7 +504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -475,7 +512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -483,7 +520,88 @@
         <v>0</v>
       </c>
     </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
latest data and updated QC criteria
</commit_message>
<xml_diff>
--- a/results/qc_check_sheets/qc_check_debrief_and_errors.xlsx
+++ b/results/qc_check_sheets/qc_check_debrief_and_errors.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\levan\GitHub\fast_schema_analysis_2\results\qc_check_sheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lb08\GitHub\fast_schema_analysis_2\results\qc_check_sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00435A46-39BD-47DF-AFC6-04D90E2316BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>participant</t>
   </si>
@@ -94,12 +93,30 @@
   </si>
   <si>
     <t>sub_020</t>
+  </si>
+  <si>
+    <t>sub_021</t>
+  </si>
+  <si>
+    <t>sub_022</t>
+  </si>
+  <si>
+    <t>sub_023</t>
+  </si>
+  <si>
+    <t>sub_024</t>
+  </si>
+  <si>
+    <t>sub_025</t>
+  </si>
+  <si>
+    <t>PC froze</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -416,20 +433,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -440,7 +457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -448,7 +465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -456,7 +473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -464,7 +481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -472,7 +489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -480,7 +497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -488,7 +505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -496,7 +513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -504,7 +521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -512,7 +529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -520,7 +537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -528,7 +545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -536,7 +553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -544,7 +561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -552,7 +569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -560,7 +577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -568,7 +585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -576,7 +593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -584,7 +601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -592,12 +609,55 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>22</v>
       </c>
       <c r="B21" t="b">
         <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" t="b">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
downloaded and analyzed the latest data
</commit_message>
<xml_diff>
--- a/results/qc_check_sheets/qc_check_debrief_and_errors.xlsx
+++ b/results/qc_check_sheets/qc_check_debrief_and_errors.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>participant</t>
   </si>
@@ -111,6 +111,15 @@
   </si>
   <si>
     <t>PC froze</t>
+  </si>
+  <si>
+    <t>sub_026</t>
+  </si>
+  <si>
+    <t>sub_027</t>
+  </si>
+  <si>
+    <t>sub_028</t>
   </si>
 </sst>
 </file>
@@ -434,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -660,6 +669,30 @@
         <v>28</v>
       </c>
     </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
latest data and analysis
</commit_message>
<xml_diff>
--- a/results/qc_check_sheets/qc_check_debrief_and_errors.xlsx
+++ b/results/qc_check_sheets/qc_check_debrief_and_errors.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lb08\GitHub\fast_schema_analysis_2\results\qc_check_sheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\levan\GitHub\fast_schema_analysis_2\results\qc_check_sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1C560AB-FB7B-4641-B425-1F61B02E4913}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>participant</t>
   </si>
@@ -120,12 +121,24 @@
   </si>
   <si>
     <t>sub_028</t>
+  </si>
+  <si>
+    <t>sub_029</t>
+  </si>
+  <si>
+    <t>unclear instructions</t>
+  </si>
+  <si>
+    <t>sub_030</t>
+  </si>
+  <si>
+    <t>extra participant</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -442,20 +455,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -466,7 +479,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -474,7 +487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -482,7 +495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -490,7 +503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -498,7 +511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -506,7 +519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -514,7 +527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -522,7 +535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -530,7 +543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -538,7 +551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -546,7 +559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -554,7 +567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -562,7 +575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -570,7 +583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -578,7 +591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -586,7 +599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -594,7 +607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -602,7 +615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -610,7 +623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -618,7 +631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -626,7 +639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -634,7 +647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -642,7 +655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -650,7 +663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -658,7 +671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -669,7 +682,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -677,7 +690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -685,11 +698,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>31</v>
       </c>
       <c r="B29" t="b">
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" t="b">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
downloaded the lastest batch of data
</commit_message>
<xml_diff>
--- a/results/qc_check_sheets/qc_check_debrief_and_errors.xlsx
+++ b/results/qc_check_sheets/qc_check_debrief_and_errors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\levan\GitHub\fast_schema_analysis_2\results\qc_check_sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D40F78F6-03BD-417B-83F2-7E125D7A2E44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E82C3081-FA52-45B6-95A1-44C130083568}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3150" yWindow="2085" windowWidth="10560" windowHeight="11205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>participant</t>
   </si>
@@ -130,6 +130,57 @@
   </si>
   <si>
     <t>sub_030</t>
+  </si>
+  <si>
+    <t>sub_031</t>
+  </si>
+  <si>
+    <t>sub_032</t>
+  </si>
+  <si>
+    <t>sub_033</t>
+  </si>
+  <si>
+    <t>sub_034</t>
+  </si>
+  <si>
+    <t>sub_035</t>
+  </si>
+  <si>
+    <t>sub_036</t>
+  </si>
+  <si>
+    <t>sub_037</t>
+  </si>
+  <si>
+    <t>sub_038</t>
+  </si>
+  <si>
+    <t>sub_039</t>
+  </si>
+  <si>
+    <t>sub_040</t>
+  </si>
+  <si>
+    <t>sub_041</t>
+  </si>
+  <si>
+    <t>sub_042</t>
+  </si>
+  <si>
+    <t>sub_043</t>
+  </si>
+  <si>
+    <t>sub_044</t>
+  </si>
+  <si>
+    <t>scroll bar issues</t>
+  </si>
+  <si>
+    <t>didn’t list all the visible items</t>
+  </si>
+  <si>
+    <t>didn’t list all the items</t>
   </si>
 </sst>
 </file>
@@ -453,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -722,6 +773,127 @@
         <v>0</v>
       </c>
     </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" t="b">
+        <v>1</v>
+      </c>
+      <c r="C33" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" t="b">
+        <v>1</v>
+      </c>
+      <c r="C34" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>39</v>
+      </c>
+      <c r="B36" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>40</v>
+      </c>
+      <c r="B37" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>41</v>
+      </c>
+      <c r="B38" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>42</v>
+      </c>
+      <c r="B39" t="b">
+        <v>1</v>
+      </c>
+      <c r="C39" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>43</v>
+      </c>
+      <c r="B40" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>44</v>
+      </c>
+      <c r="B41" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>45</v>
+      </c>
+      <c r="B42" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>46</v>
+      </c>
+      <c r="B43" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>47</v>
+      </c>
+      <c r="B44" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>48</v>
+      </c>
+      <c r="B45" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
latest batch and analysis
</commit_message>
<xml_diff>
--- a/results/qc_check_sheets/qc_check_debrief_and_errors.xlsx
+++ b/results/qc_check_sheets/qc_check_debrief_and_errors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\levan\GitHub\fast_schema_analysis_2\results\qc_check_sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E82C3081-FA52-45B6-95A1-44C130083568}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61533F15-CB89-46F0-941C-9B3D0E680277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>participant</t>
   </si>
@@ -181,6 +181,15 @@
   </si>
   <si>
     <t>didn’t list all the items</t>
+  </si>
+  <si>
+    <t>sub_045</t>
+  </si>
+  <si>
+    <t>sub_046</t>
+  </si>
+  <si>
+    <t>sub_047</t>
   </si>
 </sst>
 </file>
@@ -504,19 +513,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C45"/>
+  <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41:B48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -527,7 +536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -535,7 +544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -543,7 +552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -551,7 +560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -559,7 +568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -567,7 +576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -575,7 +584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -583,7 +592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -591,7 +600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -599,7 +608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -607,7 +616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -615,7 +624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -623,7 +632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -631,7 +640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -639,7 +648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -647,7 +656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -655,7 +664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -663,7 +672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -671,7 +680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -679,7 +688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -687,7 +696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -695,7 +704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -703,7 +712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -711,7 +720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -719,7 +728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -730,7 +739,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -738,7 +747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -746,7 +755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -754,7 +763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>32</v>
       </c>
@@ -765,7 +774,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>34</v>
       </c>
@@ -773,7 +782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>35</v>
       </c>
@@ -781,7 +790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>36</v>
       </c>
@@ -792,7 +801,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>37</v>
       </c>
@@ -803,7 +812,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>38</v>
       </c>
@@ -811,7 +820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>39</v>
       </c>
@@ -819,7 +828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>40</v>
       </c>
@@ -827,7 +836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>41</v>
       </c>
@@ -835,7 +844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>42</v>
       </c>
@@ -846,7 +855,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>43</v>
       </c>
@@ -854,7 +863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>44</v>
       </c>
@@ -862,7 +871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>45</v>
       </c>
@@ -870,7 +879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>46</v>
       </c>
@@ -878,7 +887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>47</v>
       </c>
@@ -886,11 +895,35 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>48</v>
       </c>
       <c r="B45" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>52</v>
+      </c>
+      <c r="B46" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>53</v>
+      </c>
+      <c r="B47" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>54</v>
+      </c>
+      <c r="B48" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>